<commit_message>
Added historic plots to extra bar plots Added requirements.txt and environment.yml
</commit_message>
<xml_diff>
--- a/output/boxplot_dls_table.xlsx
+++ b/output/boxplot_dls_table.xlsx
@@ -675,7 +675,7 @@
         <v>2.537908496732026</v>
       </c>
       <c r="K5" t="n">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="6">
@@ -863,7 +863,7 @@
         <v>2.894117647058823</v>
       </c>
       <c r="K9" t="n">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="10">
@@ -910,7 +910,7 @@
         <v>4.230718954248366</v>
       </c>
       <c r="K10" t="n">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="11">
@@ -1004,7 +1004,7 @@
         <v>3.680392156862745</v>
       </c>
       <c r="K12" t="n">
-        <v>644</v>
+        <v>645</v>
       </c>
     </row>
     <row r="13">
@@ -1098,7 +1098,7 @@
         <v>2.347407407407407</v>
       </c>
       <c r="K14" t="n">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="15">
@@ -1145,7 +1145,7 @@
         <v>2.305816993464052</v>
       </c>
       <c r="K15" t="n">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="16">
@@ -1380,7 +1380,7 @@
         <v>1.045025</v>
       </c>
       <c r="K20" t="n">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="21">
@@ -1474,7 +1474,7 @@
         <v>1.380344</v>
       </c>
       <c r="K22" t="n">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="23">
@@ -1662,7 +1662,7 @@
         <v>1.182932</v>
       </c>
       <c r="K26" t="n">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="27">
@@ -2034,7 +2034,7 @@
         <v>2.766</v>
       </c>
       <c r="K34" t="n">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="35">
@@ -2128,7 +2128,7 @@
         <v>2.886666666666666</v>
       </c>
       <c r="K36" t="n">
-        <v>729</v>
+        <v>730</v>
       </c>
     </row>
     <row r="37">
@@ -2269,7 +2269,7 @@
         <v>5.341365461847389</v>
       </c>
       <c r="K39" t="n">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="40">
@@ -2410,7 +2410,7 @@
         <v>0</v>
       </c>
       <c r="K42" t="n">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added lined bars for "international" values in mobility parameters; Corrected error copy-on-slice
</commit_message>
<xml_diff>
--- a/output/boxplot_dls_table.xlsx
+++ b/output/boxplot_dls_table.xlsx
@@ -2350,17 +2350,17 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>g/cap/day</t>
+          <t>kg/cap/day</t>
         </is>
       </c>
       <c r="H41" t="n">
-        <v>42.86</v>
+        <v>0.04</v>
       </c>
       <c r="I41" t="n">
         <v>62.25</v>
       </c>
       <c r="J41" t="n">
-        <v>0.6885140562248996</v>
+        <v>0.000642570281124498</v>
       </c>
       <c r="K41" t="n">
         <v>127</v>

</xml_diff>